<commit_message>
Add "Health work force with Part Time Contract in total" dataElement
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_6.xlsx
+++ b/templates/NHWA_Module_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Garza/dev/eyeseetea/WHO/excel-data-import-app/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943125F2-0BC5-3042-9727-9FC114CC01CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA053882-9DF2-FD4A-BD17-7E95D2EC8A5D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="391" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characteristics" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="800">
   <si>
     <t xml:space="preserve">NATIONAL  HEALTH WORKFORCE ACCOUNTS DATA </t>
   </si>
@@ -2516,7 +2516,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -2566,30 +2566,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -2738,9 +2716,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -2759,18 +2734,23 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2793,8 +2773,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2802,29 +2800,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -4061,8 +4039,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BZ250"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4088,21 +4066,21 @@
     <col min="34" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="2:34" ht="23" x14ac:dyDescent="0.2">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -4128,21 +4106,21 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="2:33" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="43" t="s">
+    <row r="2" spans="2:34" ht="23" x14ac:dyDescent="0.2">
+      <c r="B2" s="45" t="s">
         <v>770</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -4169,7 +4147,7 @@
         <v>202</v>
       </c>
       <c r="AC2" s="4">
-        <f t="shared" ref="AC2:AE67" si="0">--ISNUMBER(IFERROR(SEARCH($V$1,Y2,1),""))</f>
+        <f t="shared" ref="AC2:AF67" si="0">--ISNUMBER(IFERROR(SEARCH($V$1,Y2,1),""))</f>
         <v>1</v>
       </c>
       <c r="AD2" s="4">
@@ -4181,7 +4159,7 @@
         <v>Algeria</v>
       </c>
     </row>
-    <row r="3" spans="2:33" ht="23" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:34" ht="23" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -4230,7 +4208,7 @@
         <v>Angola</v>
       </c>
     </row>
-    <row r="4" spans="2:33" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
@@ -4270,7 +4248,7 @@
         <v>Benin</v>
       </c>
     </row>
-    <row r="5" spans="2:33" ht="23" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:34" ht="23" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
@@ -4313,17 +4291,17 @@
         <v>Botswana</v>
       </c>
     </row>
-    <row r="6" spans="2:33" ht="23" x14ac:dyDescent="0.2">
-      <c r="B6" s="45" t="s">
+    <row r="6" spans="2:34" ht="23" x14ac:dyDescent="0.2">
+      <c r="B6" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="49" t="s">
         <v>765</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>766</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="30"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -4334,11 +4312,11 @@
       <c r="M6" s="2"/>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="46"/>
+      <c r="S6" s="46"/>
+      <c r="T6" s="46"/>
       <c r="Y6" s="4" t="s">
         <v>17</v>
       </c>
@@ -4364,11 +4342,11 @@
         <v>Burkina Faso</v>
       </c>
     </row>
-    <row r="7" spans="2:33" ht="23" x14ac:dyDescent="0.2">
-      <c r="B7" s="45"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="31"/>
+    <row r="7" spans="2:34" ht="23" x14ac:dyDescent="0.2">
+      <c r="B7" s="47"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -4409,15 +4387,15 @@
         <v>Burundi</v>
       </c>
     </row>
-    <row r="8" spans="2:33" ht="23" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:34" ht="23" x14ac:dyDescent="0.2">
       <c r="B8" s="21">
         <v>1</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>771</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="33"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -4458,7 +4436,7 @@
         <v>Cabo Verde</v>
       </c>
     </row>
-    <row r="9" spans="2:33" ht="23" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:34" ht="23" x14ac:dyDescent="0.2">
       <c r="B9" s="24"/>
       <c r="C9" s="25"/>
       <c r="D9" s="24"/>
@@ -4503,7 +4481,7 @@
         <v>Cameroon</v>
       </c>
     </row>
-    <row r="10" spans="2:33" ht="23" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:34" ht="23" x14ac:dyDescent="0.2">
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="2"/>
@@ -4548,103 +4526,107 @@
         <v>Central African Republic</v>
       </c>
     </row>
-    <row r="11" spans="2:33" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="45" t="s">
+    <row r="11" spans="2:34" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="48" t="s">
         <v>772</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="57" t="s">
         <v>773</v>
       </c>
-      <c r="F11" s="49"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="41" t="s">
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="43" t="s">
         <v>774</v>
       </c>
-      <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
       <c r="R11" s="19"/>
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
       <c r="V11" s="19"/>
-      <c r="AA11" s="4" t="s">
+      <c r="W11" s="19"/>
+      <c r="AB11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AB11" s="4" t="s">
+      <c r="AC11" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="AC11" s="4" t="s">
+      <c r="AD11" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="AD11" s="4" t="s">
+      <c r="AE11" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AE11" s="4">
+      <c r="AF11" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AF11" s="4">
-        <f>IF(AE11=1,COUNTIF($AC$2:AC11,1),"")</f>
+      <c r="AG11" s="4">
+        <f>IF(AF11=1,COUNTIF($AC$2:AC11,1),"")</f>
         <v>9</v>
       </c>
-      <c r="AG11" s="4" t="str">
+      <c r="AH11" s="4" t="str">
         <f>IFERROR(INDEX($Y$2:$Y$250,MATCH(ROWS($AD$2:AD11),$AD$2:$AD$250,0)),"")</f>
         <v>Gambia</v>
       </c>
     </row>
-    <row r="12" spans="2:33" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="30" t="s">
+    <row r="12" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="40" t="s">
+        <v>789</v>
+      </c>
+      <c r="F12" s="40" t="s">
         <v>784</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="G12" s="28" t="s">
         <v>785</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="H12" s="28" t="s">
         <v>786</v>
       </c>
-      <c r="H12" s="42"/>
-      <c r="P12" s="19"/>
+      <c r="I12" s="44"/>
       <c r="Q12" s="19"/>
       <c r="R12" s="19"/>
       <c r="S12" s="19"/>
       <c r="T12" s="19"/>
       <c r="U12" s="19"/>
       <c r="V12" s="19"/>
-      <c r="AA12" s="4" t="s">
+      <c r="W12" s="19"/>
+      <c r="AB12" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="AB12" s="4" t="s">
+      <c r="AC12" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="AC12" s="4" t="s">
+      <c r="AD12" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="AD12" s="4" t="s">
+      <c r="AE12" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AE12" s="4">
+      <c r="AF12" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AF12" s="4">
-        <f>IF(AE12=1,COUNTIF($AC$2:AC12,1),"")</f>
+      <c r="AG12" s="4">
+        <f>IF(AF12=1,COUNTIF($AC$2:AC12,1),"")</f>
         <v>9</v>
       </c>
-      <c r="AG12" s="4" t="str">
+      <c r="AH12" s="4" t="str">
         <f>IFERROR(INDEX($Y$2:$Y$250,MATCH(ROWS($AD$2:AD12),$AD$2:$AD$250,0)),"")</f>
         <v>Ghana</v>
       </c>
     </row>
-    <row r="13" spans="2:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="7">
         <v>1</v>
       </c>
@@ -4656,39 +4638,40 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-      <c r="P13" s="19"/>
+      <c r="I13" s="10"/>
       <c r="Q13" s="19"/>
       <c r="R13" s="19"/>
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
       <c r="U13" s="19"/>
       <c r="V13" s="19"/>
-      <c r="AA13" s="4" t="s">
+      <c r="W13" s="19"/>
+      <c r="AB13" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="AB13" s="4" t="s">
+      <c r="AC13" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="AC13" s="4" t="s">
+      <c r="AD13" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="AD13" s="4" t="s">
+      <c r="AE13" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AE13" s="4">
+      <c r="AF13" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AF13" s="4">
-        <f>IF(AE13=1,COUNTIF($AC$2:AC13,1),"")</f>
+      <c r="AG13" s="4">
+        <f>IF(AF13=1,COUNTIF($AC$2:AC13,1),"")</f>
         <v>9</v>
       </c>
-      <c r="AG13" s="4" t="str">
+      <c r="AH13" s="4" t="str">
         <f>IFERROR(INDEX($Y$2:$Y$250,MATCH(ROWS($AD$2:AD13),$AD$2:$AD$250,0)),"")</f>
         <v>Guinea</v>
       </c>
     </row>
-    <row r="14" spans="2:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="7">
         <v>2</v>
       </c>
@@ -4700,39 +4683,40 @@
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
-      <c r="P14" s="19"/>
+      <c r="I14" s="10"/>
       <c r="Q14" s="19"/>
       <c r="R14" s="19"/>
       <c r="S14" s="19"/>
       <c r="T14" s="19"/>
       <c r="U14" s="19"/>
       <c r="V14" s="19"/>
-      <c r="AA14" s="4" t="s">
+      <c r="W14" s="19"/>
+      <c r="AB14" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="AB14" s="4" t="s">
+      <c r="AC14" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="AC14" s="4" t="s">
+      <c r="AD14" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="AD14" s="4" t="s">
+      <c r="AE14" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AE14" s="4">
+      <c r="AF14" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AF14" s="4">
-        <f>IF(AE14=1,COUNTIF($AC$2:AC14,1),"")</f>
+      <c r="AG14" s="4">
+        <f>IF(AF14=1,COUNTIF($AC$2:AC14,1),"")</f>
         <v>9</v>
       </c>
-      <c r="AG14" s="4" t="str">
+      <c r="AH14" s="4" t="str">
         <f>IFERROR(INDEX($Y$2:$Y$250,MATCH(ROWS($AD$2:AD14),$AD$2:$AD$250,0)),"")</f>
         <v>Guinea-Bissau</v>
       </c>
     </row>
-    <row r="15" spans="2:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="7">
         <v>3</v>
       </c>
@@ -4744,39 +4728,40 @@
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
-      <c r="P15" s="20"/>
+      <c r="I15" s="10"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="20"/>
-      <c r="S15" s="19"/>
+      <c r="S15" s="20"/>
       <c r="T15" s="19"/>
       <c r="U15" s="19"/>
       <c r="V15" s="19"/>
-      <c r="AA15" s="4" t="s">
+      <c r="W15" s="19"/>
+      <c r="AB15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AB15" s="4" t="s">
+      <c r="AC15" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="AC15" s="4" t="s">
+      <c r="AD15" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="AD15" s="4" t="s">
+      <c r="AE15" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AE15" s="4">
+      <c r="AF15" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AF15" s="4">
-        <f>IF(AE15=1,COUNTIF($AC$2:AC15,1),"")</f>
+      <c r="AG15" s="4">
+        <f>IF(AF15=1,COUNTIF($AC$2:AC15,1),"")</f>
         <v>9</v>
       </c>
-      <c r="AG15" s="4" t="str">
+      <c r="AH15" s="4" t="str">
         <f>IFERROR(INDEX($Y$2:$Y$250,MATCH(ROWS($AD$2:AD15),$AD$2:$AD$250,0)),"")</f>
         <v>Kenya</v>
       </c>
     </row>
-    <row r="16" spans="2:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="7">
         <v>4</v>
       </c>
@@ -4788,32 +4773,33 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
-      <c r="AA16" s="4" t="s">
+      <c r="I16" s="10"/>
+      <c r="AB16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AB16" s="4" t="s">
+      <c r="AC16" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="AC16" s="4" t="s">
+      <c r="AD16" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="AD16" s="4" t="s">
+      <c r="AE16" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AE16" s="4">
+      <c r="AF16" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AF16" s="4">
-        <f>IF(AE16=1,COUNTIF($AC$2:AC16,1),"")</f>
+      <c r="AG16" s="4">
+        <f>IF(AF16=1,COUNTIF($AC$2:AC16,1),"")</f>
         <v>9</v>
       </c>
-      <c r="AG16" s="4" t="str">
+      <c r="AH16" s="4" t="str">
         <f>IFERROR(INDEX($Y$2:$Y$250,MATCH(ROWS($AD$2:AD16),$AD$2:$AD$250,0)),"")</f>
         <v>Lesotho</v>
       </c>
     </row>
-    <row r="17" spans="2:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="7">
         <v>5</v>
       </c>
@@ -4825,32 +4811,33 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-      <c r="AA17" s="4" t="s">
+      <c r="I17" s="10"/>
+      <c r="AB17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AB17" s="4" t="s">
+      <c r="AC17" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="AC17" s="4" t="s">
+      <c r="AD17" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="AD17" s="4" t="s">
+      <c r="AE17" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AE17" s="4">
+      <c r="AF17" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AF17" s="4">
-        <f>IF(AE17=1,COUNTIF($AC$2:AC17,1),"")</f>
+      <c r="AG17" s="4">
+        <f>IF(AF17=1,COUNTIF($AC$2:AC17,1),"")</f>
         <v>9</v>
       </c>
-      <c r="AG17" s="4" t="str">
+      <c r="AH17" s="4" t="str">
         <f>IFERROR(INDEX($Y$2:$Y$250,MATCH(ROWS($AD$2:AD17),$AD$2:$AD$250,0)),"")</f>
         <v>Liberia</v>
       </c>
     </row>
-    <row r="18" spans="2:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="7">
         <v>6</v>
       </c>
@@ -4862,32 +4849,33 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
-      <c r="AA18" s="4" t="s">
+      <c r="I18" s="10"/>
+      <c r="AB18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AB18" s="4" t="s">
+      <c r="AC18" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="AC18" s="4" t="s">
+      <c r="AD18" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="AD18" s="4" t="s">
+      <c r="AE18" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AE18" s="4">
+      <c r="AF18" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AF18" s="4">
-        <f>IF(AE18=1,COUNTIF($AC$2:AC18,1),"")</f>
+      <c r="AG18" s="4">
+        <f>IF(AF18=1,COUNTIF($AC$2:AC18,1),"")</f>
         <v>9</v>
       </c>
-      <c r="AG18" s="4" t="str">
+      <c r="AH18" s="4" t="str">
         <f>IFERROR(INDEX($Y$2:$Y$250,MATCH(ROWS($AD$2:AD18),$AD$2:$AD$250,0)),"")</f>
         <v>Madagascar</v>
       </c>
     </row>
-    <row r="19" spans="2:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="7">
         <v>7</v>
       </c>
@@ -4899,32 +4887,33 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
-      <c r="AA19" s="4" t="s">
+      <c r="I19" s="10"/>
+      <c r="AB19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB19" s="4" t="s">
+      <c r="AC19" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="AC19" s="4" t="s">
+      <c r="AD19" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="AD19" s="4" t="s">
+      <c r="AE19" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AE19" s="4">
+      <c r="AF19" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AF19" s="4">
-        <f>IF(AE19=1,COUNTIF($AC$2:AC19,1),"")</f>
+      <c r="AG19" s="4">
+        <f>IF(AF19=1,COUNTIF($AC$2:AC19,1),"")</f>
         <v>9</v>
       </c>
-      <c r="AG19" s="4" t="str">
+      <c r="AH19" s="4" t="str">
         <f>IFERROR(INDEX($Y$2:$Y$250,MATCH(ROWS($AD$2:AD19),$AD$2:$AD$250,0)),"")</f>
         <v>Malawi</v>
       </c>
     </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y20" s="4" t="s">
         <v>27</v>
       </c>
@@ -4950,7 +4939,7 @@
         <v>Mali</v>
       </c>
     </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y21" s="4" t="s">
         <v>28</v>
       </c>
@@ -4976,7 +4965,7 @@
         <v>Mauritania</v>
       </c>
     </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y22" s="4" t="s">
         <v>29</v>
       </c>
@@ -5002,7 +4991,7 @@
         <v>Mauritius</v>
       </c>
     </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y23" s="4" t="s">
         <v>30</v>
       </c>
@@ -5028,7 +5017,7 @@
         <v>Mozambique</v>
       </c>
     </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y24" s="4" t="s">
         <v>31</v>
       </c>
@@ -5054,7 +5043,7 @@
         <v>Namibia</v>
       </c>
     </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y25" s="4" t="s">
         <v>32</v>
       </c>
@@ -5080,7 +5069,7 @@
         <v>Niger</v>
       </c>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y26" s="4" t="s">
         <v>33</v>
       </c>
@@ -5106,7 +5095,7 @@
         <v>Nigeria</v>
       </c>
     </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y27" s="4" t="s">
         <v>34</v>
       </c>
@@ -5132,7 +5121,7 @@
         <v>Rwanda</v>
       </c>
     </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y28" s="4" t="s">
         <v>35</v>
       </c>
@@ -5158,7 +5147,7 @@
         <v>Sao Tome and Principe</v>
       </c>
     </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y29" s="4" t="s">
         <v>36</v>
       </c>
@@ -5184,7 +5173,7 @@
         <v>Senegal</v>
       </c>
     </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y30" s="4" t="s">
         <v>37</v>
       </c>
@@ -5210,7 +5199,7 @@
         <v>Seychelles</v>
       </c>
     </row>
-    <row r="31" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y31" s="4" t="s">
         <v>38</v>
       </c>
@@ -5236,7 +5225,7 @@
         <v>Sierra Leone</v>
       </c>
     </row>
-    <row r="32" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:34" x14ac:dyDescent="0.2">
       <c r="Y32" s="4" t="s">
         <v>39</v>
       </c>
@@ -10951,10 +10940,10 @@
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="I4 S11:T15 E13:O19 D18:D19 D13:D16 P11:R14 N8:P10 Q8:R10" name="Range1"/>
+    <protectedRange sqref="I4 T11:U15 F13:P19 D18:D19 D13:D16 Q11:S14 N8:P10 Q8:R10 E13:E16 E18:E19" name="Range1"/>
   </protectedRanges>
   <mergeCells count="12">
-    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="S6:T6"/>
@@ -10964,11 +10953,11 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E11:G11"/>
     <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E11:H11"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8 D13:H19" xr:uid="{831435B8-54B8-C540-BEC3-C109BE66913C}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8 D13:I19" xr:uid="{831435B8-54B8-C540-BEC3-C109BE66913C}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -10983,7 +10972,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17:F18"/>
     </sheetView>
   </sheetViews>
@@ -11008,36 +10997,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
     </row>
     <row r="2" spans="2:19" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="45" t="s">
         <v>770</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
       <c r="N2" s="14" t="e">
         <f>Characteristics!V2</f>
         <v>#N/A</v>
@@ -11102,16 +11091,16 @@
       </c>
     </row>
     <row r="7" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="47" t="s">
         <v>776</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="47" t="s">
         <v>777</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="47" t="s">
         <v>799</v>
       </c>
       <c r="N7" s="14" t="s">
@@ -11119,10 +11108,10 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
       <c r="O8" s="14"/>
       <c r="P8" s="4" t="s">
         <v>767</v>
@@ -11186,13 +11175,13 @@
       </c>
     </row>
     <row r="11" spans="2:19" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="34">
+      <c r="B11" s="33">
         <v>3</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="34" t="s">
         <v>779</v>
       </c>
-      <c r="D11" s="36"/>
+      <c r="D11" s="35"/>
       <c r="E11" s="26"/>
       <c r="N11" s="14">
         <v>1</v>
@@ -11208,18 +11197,18 @@
       </c>
     </row>
     <row r="12" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
     </row>
     <row r="14" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="47" t="s">
         <v>776</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="50" t="s">
         <v>789</v>
       </c>
       <c r="E14" s="54" t="s">
@@ -11230,9 +11219,9 @@
       <c r="H14" s="56"/>
     </row>
     <row r="15" spans="2:19" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="52"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="29" t="s">
         <v>791</v>
       </c>
@@ -11247,7 +11236,7 @@
       </c>
     </row>
     <row r="16" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="40">
+      <c r="B16" s="39">
         <v>1</v>
       </c>
       <c r="C16" s="23" t="s">
@@ -11263,52 +11252,61 @@
       <c r="B17" s="53"/>
       <c r="C17" s="53"/>
       <c r="D17" s="53"/>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="50" t="s">
         <v>795</v>
       </c>
-      <c r="F17" s="51" t="s">
+      <c r="F17" s="50" t="s">
         <v>796</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="53"/>
       <c r="C18" s="53"/>
       <c r="D18" s="53"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
     </row>
     <row r="19" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="40">
+      <c r="B19" s="39">
         <v>2</v>
       </c>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="52" t="s">
         <v>797</v>
       </c>
-      <c r="D19" s="57"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="40">
+      <c r="B20" s="39">
         <v>3</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="52" t="s">
         <v>798</v>
       </c>
-      <c r="D20" s="57"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="B17:B18"/>
@@ -11316,15 +11314,6 @@
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16 E16 F16 G16 H16 E19:F19 G19:H19 G20:H20 E20:F20" xr:uid="{FDC70E15-49BA-094D-9C58-0F6BF1E6C1E0}">
@@ -11437,32 +11426,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="2:18" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="45" t="s">
         <v>770</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -11528,16 +11517,16 @@
       </c>
     </row>
     <row r="7" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="48" t="s">
         <v>781</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="48" t="s">
         <v>799</v>
       </c>
       <c r="M7" s="4" t="s">
@@ -11548,10 +11537,10 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
       <c r="O8" s="14"/>
       <c r="P8" s="4" t="s">
         <v>767</v>
@@ -11754,26 +11743,26 @@
       <c r="O17" s="14"/>
     </row>
     <row r="18" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="49" t="s">
         <v>765</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="50" t="s">
         <v>766</v>
       </c>
-      <c r="E18" s="51" t="s">
+      <c r="E18" s="50" t="s">
         <v>799</v>
       </c>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="45"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>

</xml_diff>

<commit_message>
Update excel and script with form changes
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_6.xlsx
+++ b/templates/NHWA_Module_6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Garza/dev/eyeseetea/WHO/excel-data-import-app/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA053882-9DF2-FD4A-BD17-7E95D2EC8A5D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559AF9CB-F76B-D74F-8B0D-A23DDA2CD08A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" tabRatio="391" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characteristics" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="797">
   <si>
     <t xml:space="preserve">NATIONAL  HEALTH WORKFORCE ACCOUNTS DATA </t>
   </si>
@@ -2350,15 +2350,6 @@
     <t>Standard working hours as per the national law</t>
   </si>
   <si>
-    <t>Standard Working Hours in a week</t>
-  </si>
-  <si>
-    <t>HWF with Part Time Contract</t>
-  </si>
-  <si>
-    <t>Self employed workers</t>
-  </si>
-  <si>
     <t>Existence of national/sub-national policies/laws for prevention of attacks on health workers</t>
   </si>
   <si>
@@ -2374,9 +2365,6 @@
     <t>Existence of national/sub-national policies/laws regulating dual practice</t>
   </si>
   <si>
-    <t>Number of violent attacks on health workers</t>
-  </si>
-  <si>
     <t>Existence of national law on regulating Working hours and conditions</t>
   </si>
   <si>
@@ -2419,19 +2407,22 @@
     <t>Patient</t>
   </si>
   <si>
-    <t>Physical attacks</t>
-  </si>
-  <si>
-    <t>Psychological attacks</t>
-  </si>
-  <si>
-    <t>Number of violent attacks on health care providers</t>
-  </si>
-  <si>
-    <t>Number of violent attacks on patients</t>
-  </si>
-  <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Standard Working Hours in a week (6-01)</t>
+  </si>
+  <si>
+    <t>Standard working hours in a week (6-01)</t>
+  </si>
+  <si>
+    <t>HWF with Part Time Contract (6-02)</t>
+  </si>
+  <si>
+    <t>Self employed workers (6-06)</t>
+  </si>
+  <si>
+    <t>Number of attacks on health-care system (6-10)</t>
   </si>
 </sst>
 </file>
@@ -2635,7 +2626,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2749,7 +2740,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2779,11 +2769,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2794,14 +2787,17 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -4039,8 +4035,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BZ250"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4048,12 +4044,12 @@
     <col min="1" max="1" width="9.1640625" style="4"/>
     <col min="2" max="2" width="10.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="53.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18" style="4" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.5" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="10" style="4" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" style="4" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" style="4" customWidth="1"/>
     <col min="11" max="15" width="9.1640625" style="4" customWidth="1"/>
     <col min="16" max="16" width="12.6640625" style="4" customWidth="1"/>
@@ -4067,20 +4063,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:34" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -4107,20 +4103,20 @@
       </c>
     </row>
     <row r="2" spans="2:34" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="44" t="s">
         <v>770</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -4292,14 +4288,14 @@
       </c>
     </row>
     <row r="6" spans="2:34" ht="23" x14ac:dyDescent="0.2">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="48" t="s">
         <v>765</v>
       </c>
-      <c r="D6" s="50" t="s">
-        <v>766</v>
+      <c r="D6" s="49" t="s">
+        <v>793</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="2"/>
@@ -4312,11 +4308,11 @@
       <c r="M6" s="2"/>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="46"/>
-      <c r="T6" s="46"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
       <c r="Y6" s="4" t="s">
         <v>17</v>
       </c>
@@ -4343,9 +4339,9 @@
       </c>
     </row>
     <row r="7" spans="2:34" ht="23" x14ac:dyDescent="0.2">
-      <c r="B7" s="47"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="51"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="50"/>
       <c r="E7" s="30"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -4527,23 +4523,23 @@
       </c>
     </row>
     <row r="11" spans="2:34" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="48" t="s">
-        <v>772</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>773</v>
-      </c>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="43" t="s">
-        <v>774</v>
+      <c r="D11" s="47" t="s">
+        <v>792</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>794</v>
+      </c>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="42" t="s">
+        <v>795</v>
       </c>
       <c r="Q11" s="19"/>
       <c r="R11" s="19"/>
@@ -4578,22 +4574,22 @@
       </c>
     </row>
     <row r="12" spans="2:34" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="40" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>786</v>
-      </c>
-      <c r="I12" s="44"/>
+        <v>782</v>
+      </c>
+      <c r="I12" s="43"/>
       <c r="Q12" s="19"/>
       <c r="R12" s="19"/>
       <c r="S12" s="19"/>
@@ -10972,8 +10968,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10997,36 +10993,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
     </row>
     <row r="2" spans="2:19" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="44" t="s">
         <v>770</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="14" t="e">
         <f>Characteristics!V2</f>
         <v>#N/A</v>
@@ -11084,46 +11080,46 @@
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
       <c r="L6" s="5"/>
       <c r="N6" s="4" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="7" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="47" t="s">
-        <v>776</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>777</v>
-      </c>
-      <c r="E7" s="47" t="s">
-        <v>799</v>
+      <c r="C7" s="46" t="s">
+        <v>773</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>774</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>791</v>
       </c>
       <c r="N7" s="14" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
       <c r="O8" s="14"/>
       <c r="P8" s="4" t="s">
         <v>767</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>768</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="39" customHeight="1" x14ac:dyDescent="0.2">
@@ -11131,7 +11127,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
@@ -11157,7 +11153,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -11179,7 +11175,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="26"/>
@@ -11202,37 +11198,37 @@
       <c r="D12" s="38"/>
     </row>
     <row r="14" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="47" t="s">
-        <v>776</v>
-      </c>
-      <c r="D14" s="50" t="s">
-        <v>789</v>
+      <c r="C14" s="46" t="s">
+        <v>773</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>785</v>
       </c>
       <c r="E14" s="54" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="F14" s="55"/>
       <c r="G14" s="55"/>
       <c r="H14" s="56"/>
     </row>
     <row r="15" spans="2:19" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="51"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="29" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
     </row>
     <row r="16" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -11240,7 +11236,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>780</v>
+        <v>796</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
@@ -11249,55 +11245,50 @@
       <c r="H16" s="26"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="50" t="s">
-        <v>795</v>
-      </c>
-      <c r="F17" s="50" t="s">
-        <v>796</v>
-      </c>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
       <c r="G18" s="30"/>
       <c r="H18" s="30"/>
     </row>
     <row r="19" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="39">
-        <v>2</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>797</v>
-      </c>
-      <c r="D19" s="52"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
       <c r="E19" s="41"/>
       <c r="F19" s="41"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="39">
-        <v>3</v>
-      </c>
-      <c r="C20" s="52" t="s">
-        <v>798</v>
-      </c>
-      <c r="D20" s="52"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="E7:E8"/>
@@ -11307,13 +11298,6 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16 E16 F16 G16 H16 E19:F19 G19:H19 G20:H20 E20:F20" xr:uid="{FDC70E15-49BA-094D-9C58-0F6BF1E6C1E0}">
@@ -11404,7 +11388,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:S21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="125" workbookViewId="0">
       <selection activeCell="L1" sqref="L1:S1048576"/>
     </sheetView>
   </sheetViews>
@@ -11426,32 +11410,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="2:18" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="44" t="s">
         <v>770</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -11513,21 +11497,21 @@
         <v>767</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="48" t="s">
-        <v>781</v>
-      </c>
-      <c r="E7" s="48" t="s">
-        <v>799</v>
+      <c r="D7" s="47" t="s">
+        <v>777</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>791</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>768</v>
@@ -11537,16 +11521,16 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
       <c r="O8" s="14"/>
       <c r="P8" s="4" t="s">
         <v>767</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="R8" s="4" t="s">
         <v>768</v>
@@ -11743,26 +11727,26 @@
       <c r="O17" s="14"/>
     </row>
     <row r="18" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="48" t="s">
         <v>765</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="49" t="s">
         <v>766</v>
       </c>
-      <c r="E18" s="50" t="s">
-        <v>799</v>
+      <c r="E18" s="49" t="s">
+        <v>791</v>
       </c>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="47"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
@@ -11771,7 +11755,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="26"/>
@@ -11788,7 +11772,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="26"/>

</xml_diff>

<commit_message>
Updates for modules 6 and 8
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_6.xlsx
+++ b/templates/NHWA_Module_6.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20350"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20351"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\EST\Excel_Data_Importer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FBA633-C6D9-404F-AA32-CE14AC10195B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533A79CA-DAAA-4778-A3CC-889B5E364217}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DNn2ED2tvDz8R2HdUrc6XR6aLxi7PHt3jXYcZD0jxFrPsDBA7xDhVMdxOKshsbgCwgXdklO6j3XC0t5iHKIwCg==" workbookSaltValue="hoPvbRWBNZzUUX5QAUaMpQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -2503,7 +2503,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2610,17 +2610,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -2632,14 +2621,12 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </right>
+      </left>
+      <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -2666,7 +2653,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2803,12 +2790,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2822,13 +2803,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2836,6 +2817,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -4221,7 +4213,7 @@
         <v>Benin</v>
       </c>
     </row>
-    <row r="5" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
@@ -4268,13 +4260,13 @@
       <c r="B6" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="46" t="s">
         <v>763</v>
       </c>
       <c r="D6" s="49" t="s">
         <v>788</v>
       </c>
-      <c r="E6" s="50"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -4317,9 +4309,9 @@
     </row>
     <row r="7" spans="2:31" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="46"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="61"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -4360,15 +4352,15 @@
         <v>Burundi</v>
       </c>
     </row>
-    <row r="8" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15">
         <v>1</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>769</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="62"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -4409,7 +4401,7 @@
         <v>Cabo Verde</v>
       </c>
     </row>
-    <row r="9" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
       <c r="D9" s="18"/>
@@ -4454,7 +4446,7 @@
         <v>Cameroon</v>
       </c>
     </row>
-    <row r="10" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="2"/>
@@ -4509,12 +4501,12 @@
       <c r="D11" s="47" t="s">
         <v>787</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="52" t="s">
         <v>789</v>
       </c>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="56"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="54"/>
       <c r="I11" s="42" t="s">
         <v>790</v>
       </c>
@@ -10912,12 +10904,12 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kaUoaCOkeIUWTbO+jsr9BK1atBw38xmfbrpsIkro64oK0OTeoYoryWqKMoQmv0IdthcExS2/57wURwwq83VKYA==" saltValue="Hds9W8lE3w8Mqf2O2eG35w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="k5WLaYVqQv4j6zpGYXQVhwccn5iD/wlID+cnpmcDkZq05rPeEJ5OltkYc+nENGaAESsICF85rEADnGjgFcOklg==" saltValue="Y0UpyvBZGiBCYwWrcKtcww==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="I4 Q8:R15 J13:M19 N8:P14" name="Range1"/>
     <protectedRange sqref="F13:I19 D13:E16 D18:E19" name="Range1_1"/>
   </protectedRanges>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
@@ -10928,12 +10920,11 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="D8:E8"/>
     <mergeCell ref="E11:H11"/>
+    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:I19" xr:uid="{1AEA519C-D6C3-4B19-BC8C-DB1A1E5CA382}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:I19 D8:E8" xr:uid="{1AEA519C-D6C3-4B19-BC8C-DB1A1E5CA382}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4" xr:uid="{C90E78D1-5234-4547-8AA5-47EF92B03D04}">
@@ -11101,7 +11092,7 @@
       <c r="C7" s="46" t="s">
         <v>770</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="55" t="s">
         <v>771</v>
       </c>
       <c r="E7" s="46" t="s">
@@ -11117,7 +11108,7 @@
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B8" s="46"/>
       <c r="C8" s="46"/>
-      <c r="D8" s="59"/>
+      <c r="D8" s="55"/>
       <c r="E8" s="46"/>
       <c r="F8" s="46"/>
       <c r="G8" s="46"/>
@@ -11144,10 +11135,10 @@
         <v>791</v>
       </c>
       <c r="D9" s="29"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
       <c r="N9" s="11">
         <v>1</v>
       </c>
@@ -11173,10 +11164,10 @@
         <v>792</v>
       </c>
       <c r="D10" s="29"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
       <c r="N10" s="11">
         <v>1</v>
       </c>
@@ -11198,10 +11189,10 @@
         <v>793</v>
       </c>
       <c r="D11" s="32"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
       <c r="N11" s="11">
         <v>1</v>
       </c>
@@ -11227,20 +11218,20 @@
       <c r="C14" s="46" t="s">
         <v>770</v>
       </c>
-      <c r="D14" s="57" t="s">
+      <c r="D14" s="56" t="s">
         <v>775</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="55" t="s">
         <v>776</v>
       </c>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="61"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="59"/>
     </row>
     <row r="15" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="46"/>
       <c r="C15" s="46"/>
-      <c r="D15" s="58"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="23" t="s">
         <v>777</v>
       </c>
@@ -11306,12 +11297,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="njO8t2UNzwLibFRM7/QfgGWZVKVcn/gHeiCHWwDTPFdW/Pju/K7pTCpOKjHRfrbNCcEYYzPWr9IIT7bp2ycbTQ==" saltValue="rbWw0nActd2GAs+GRzK7kw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="13">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="E7:H8"/>
     <mergeCell ref="E9:H9"/>
     <mergeCell ref="E10:H10"/>
     <mergeCell ref="E11:H11"/>
@@ -11319,6 +11304,12 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="E7:H8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16:H16 E19:H20" xr:uid="{BB8CFBDE-3701-4918-8149-6D661D113196}">
@@ -11568,11 +11559,11 @@
         <v>4</v>
       </c>
       <c r="D9" s="21"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
       <c r="N9" s="11">
         <v>1</v>
       </c>
@@ -11598,11 +11589,11 @@
         <v>782</v>
       </c>
       <c r="D10" s="21"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
       <c r="N10" s="11">
         <v>1</v>
       </c>
@@ -11628,11 +11619,11 @@
         <v>783</v>
       </c>
       <c r="D11" s="21"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
       <c r="N11" s="11">
         <v>1</v>
       </c>
@@ -11658,11 +11649,11 @@
         <v>5</v>
       </c>
       <c r="D12" s="21"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
       <c r="N12" s="11">
         <v>1</v>
       </c>
@@ -11688,11 +11679,11 @@
         <v>6</v>
       </c>
       <c r="D13" s="21"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
       <c r="N13" s="11">
         <v>1</v>
       </c>
@@ -11718,11 +11709,11 @@
         <v>7</v>
       </c>
       <c r="D14" s="21"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
       <c r="N14" s="11">
         <v>1</v>
       </c>
@@ -11748,11 +11739,11 @@
         <v>8</v>
       </c>
       <c r="D15" s="21"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
       <c r="N15" s="11">
         <v>1</v>
       </c>
@@ -11785,7 +11776,7 @@
       <c r="C18" s="48" t="s">
         <v>763</v>
       </c>
-      <c r="D18" s="57" t="s">
+      <c r="D18" s="56" t="s">
         <v>764</v>
       </c>
       <c r="E18" s="46" t="s">
@@ -11801,7 +11792,7 @@
     <row r="19" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="46"/>
       <c r="C19" s="48"/>
-      <c r="D19" s="58"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="46"/>
       <c r="F19" s="46"/>
       <c r="G19" s="46"/>
@@ -11818,11 +11809,11 @@
         <v>795</v>
       </c>
       <c r="D20" s="21"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
       <c r="N20" s="11">
         <v>1</v>
       </c>
@@ -11839,11 +11830,11 @@
         <v>796</v>
       </c>
       <c r="D21" s="21"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
       <c r="N21" s="11">
         <v>1</v>
       </c>
@@ -11864,11 +11855,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="U6zHl81zHEJFHtcGEmWN7K/Nl7VQXEMwqrV3P/k+2/k78IMzbhKEqDtEEXpRJWX9nJ1s2RpNkh1Lzmte3WBCkg==" saltValue="maxO/YNHiX/BdQ39wuXx1g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="19">
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E18:I19"/>
-    <mergeCell ref="E20:I20"/>
     <mergeCell ref="E21:I21"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="B1:I1"/>
@@ -11883,6 +11869,11 @@
     <mergeCell ref="E10:I10"/>
     <mergeCell ref="E11:I11"/>
     <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E18:I19"/>
+    <mergeCell ref="E20:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>